<commit_message>
fix client payment report
</commit_message>
<xml_diff>
--- a/resources/import/followups_report.xlsx
+++ b/resources/import/followups_report.xlsx
@@ -11,9 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>OWNER</t>
+  </si>
+  <si>
+    <t>CLIENT</t>
   </si>
   <si>
     <t>LINE OF BUSINESS</t>
@@ -309,12 +312,13 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="17.5"/>
-    <col customWidth="1" min="2" max="2" width="20.5"/>
-    <col customWidth="1" min="3" max="3" width="27.13"/>
-    <col customWidth="1" min="4" max="4" width="21.75"/>
-    <col customWidth="1" min="5" max="5" width="19.0"/>
-    <col customWidth="1" min="6" max="6" width="28.88"/>
-    <col customWidth="1" min="7" max="7" width="62.38"/>
+    <col customWidth="1" min="2" max="2" width="27.5"/>
+    <col customWidth="1" min="3" max="3" width="20.5"/>
+    <col customWidth="1" min="4" max="4" width="27.13"/>
+    <col customWidth="1" min="5" max="5" width="21.75"/>
+    <col customWidth="1" min="6" max="6" width="19.0"/>
+    <col customWidth="1" min="7" max="7" width="28.88"/>
+    <col customWidth="1" min="8" max="8" width="62.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -339,6 +343,9 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>